<commit_message>
19.10.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/October/All Details/19.10.2020/MC Bank Statement Sep-2020.xlsx
+++ b/2020/October/All Details/19.10.2020/MC Bank Statement Sep-2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="599" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Oct 2020" sheetId="7" r:id="rId1"/>
@@ -153,12 +153,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="F22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Hirok Accident Doctor Cost+ CC Care Appayon= 988+150
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="223">
   <si>
     <t>Date</t>
   </si>
@@ -802,12 +827,6 @@
     <t>14.10.2020</t>
   </si>
   <si>
-    <t>Bhai Bhai Bagha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rimi Tel </t>
-  </si>
-  <si>
     <t>B=Molla Enterprise</t>
   </si>
   <si>
@@ -823,10 +842,16 @@
     <t>18.10.2020</t>
   </si>
   <si>
-    <t>Date: 18.10.2020</t>
+    <t>Noman Tel</t>
   </si>
   <si>
-    <t>Noman Tel</t>
+    <t>19.10.2020</t>
+  </si>
+  <si>
+    <t>Date: 19.10.2020</t>
+  </si>
+  <si>
+    <t>i99=DSR</t>
   </si>
 </sst>
 </file>
@@ -3724,7 +3749,7 @@
   <dimension ref="A1:H85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4038,7 +4063,7 @@
     <row r="19" spans="1:8" ht="12.75" customHeight="1">
       <c r="A19" s="35"/>
       <c r="B19" s="40" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C19" s="39">
         <v>710000</v>
@@ -4057,7 +4082,7 @@
     <row r="20" spans="1:8">
       <c r="A20" s="35"/>
       <c r="B20" s="40" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C20" s="39">
         <v>0</v>
@@ -4076,7 +4101,7 @@
     <row r="21" spans="1:8">
       <c r="A21" s="35"/>
       <c r="B21" s="40" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C21" s="39">
         <v>1570000</v>
@@ -4094,12 +4119,18 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="35"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
+      <c r="B22" s="40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C22" s="39">
+        <v>500000</v>
+      </c>
+      <c r="D22" s="290">
+        <v>400000</v>
+      </c>
       <c r="E22" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="2"/>
@@ -4112,7 +4143,7 @@
       <c r="D23" s="39"/>
       <c r="E23" s="41">
         <f>E22+C23-D23</f>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F23" s="31"/>
       <c r="G23" s="2"/>
@@ -4125,7 +4156,7 @@
       <c r="D24" s="39"/>
       <c r="E24" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F24" s="31"/>
       <c r="G24" s="2"/>
@@ -4138,7 +4169,7 @@
       <c r="D25" s="39"/>
       <c r="E25" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F25" s="31"/>
       <c r="G25" s="2"/>
@@ -4151,7 +4182,7 @@
       <c r="D26" s="39"/>
       <c r="E26" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F26" s="31"/>
       <c r="G26" s="2"/>
@@ -4164,7 +4195,7 @@
       <c r="D27" s="39"/>
       <c r="E27" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F27" s="31"/>
       <c r="G27" s="2"/>
@@ -4177,7 +4208,7 @@
       <c r="D28" s="39"/>
       <c r="E28" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F28" s="31"/>
       <c r="G28" s="2"/>
@@ -4190,7 +4221,7 @@
       <c r="D29" s="39"/>
       <c r="E29" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F29" s="31"/>
       <c r="G29" s="2"/>
@@ -4203,7 +4234,7 @@
       <c r="D30" s="39"/>
       <c r="E30" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F30" s="31"/>
       <c r="G30" s="2"/>
@@ -4216,7 +4247,7 @@
       <c r="D31" s="39"/>
       <c r="E31" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F31" s="31"/>
       <c r="G31" s="2"/>
@@ -4229,7 +4260,7 @@
       <c r="D32" s="39"/>
       <c r="E32" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F32" s="31"/>
       <c r="G32" s="2"/>
@@ -4242,7 +4273,7 @@
       <c r="D33" s="42"/>
       <c r="E33" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F33" s="31"/>
       <c r="G33" s="2"/>
@@ -4255,7 +4286,7 @@
       <c r="D34" s="39"/>
       <c r="E34" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F34" s="31"/>
       <c r="G34" s="2"/>
@@ -4268,7 +4299,7 @@
       <c r="D35" s="39"/>
       <c r="E35" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F35" s="31"/>
       <c r="G35" s="2"/>
@@ -4281,7 +4312,7 @@
       <c r="D36" s="39"/>
       <c r="E36" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F36" s="31"/>
       <c r="G36" s="2"/>
@@ -4294,7 +4325,7 @@
       <c r="D37" s="39"/>
       <c r="E37" s="41">
         <f t="shared" si="0"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F37" s="31"/>
       <c r="G37" s="2"/>
@@ -4307,7 +4338,7 @@
       <c r="D38" s="39"/>
       <c r="E38" s="41">
         <f t="shared" ref="E38:E69" si="1">E37+C38-D38</f>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F38" s="31"/>
       <c r="G38" s="2"/>
@@ -4320,7 +4351,7 @@
       <c r="D39" s="39"/>
       <c r="E39" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F39" s="31"/>
       <c r="G39" s="2"/>
@@ -4333,7 +4364,7 @@
       <c r="D40" s="39"/>
       <c r="E40" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F40" s="31"/>
       <c r="G40" s="2"/>
@@ -4346,7 +4377,7 @@
       <c r="D41" s="39"/>
       <c r="E41" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F41" s="31"/>
       <c r="G41" s="2"/>
@@ -4359,7 +4390,7 @@
       <c r="D42" s="39"/>
       <c r="E42" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F42" s="31"/>
       <c r="G42" s="2"/>
@@ -4372,7 +4403,7 @@
       <c r="D43" s="39"/>
       <c r="E43" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F43" s="31"/>
       <c r="G43" s="2"/>
@@ -4385,7 +4416,7 @@
       <c r="D44" s="39"/>
       <c r="E44" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F44" s="31"/>
       <c r="G44" s="2"/>
@@ -4398,7 +4429,7 @@
       <c r="D45" s="39"/>
       <c r="E45" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F45" s="31"/>
       <c r="G45" s="2"/>
@@ -4411,7 +4442,7 @@
       <c r="D46" s="39"/>
       <c r="E46" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F46" s="31"/>
       <c r="G46" s="2"/>
@@ -4424,7 +4455,7 @@
       <c r="D47" s="39"/>
       <c r="E47" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F47" s="31"/>
       <c r="G47" s="2"/>
@@ -4437,7 +4468,7 @@
       <c r="D48" s="39"/>
       <c r="E48" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F48" s="31"/>
       <c r="G48" s="2"/>
@@ -4449,7 +4480,7 @@
       <c r="D49" s="39"/>
       <c r="E49" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F49" s="31"/>
       <c r="G49" s="2"/>
@@ -4461,7 +4492,7 @@
       <c r="D50" s="39"/>
       <c r="E50" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F50" s="31"/>
       <c r="G50" s="2"/>
@@ -4473,7 +4504,7 @@
       <c r="D51" s="39"/>
       <c r="E51" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F51" s="31"/>
       <c r="G51" s="2"/>
@@ -4485,7 +4516,7 @@
       <c r="D52" s="39"/>
       <c r="E52" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F52" s="31"/>
       <c r="G52" s="2"/>
@@ -4497,7 +4528,7 @@
       <c r="D53" s="39"/>
       <c r="E53" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F53" s="31"/>
       <c r="G53" s="2"/>
@@ -4509,7 +4540,7 @@
       <c r="D54" s="39"/>
       <c r="E54" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F54" s="31"/>
       <c r="G54" s="2"/>
@@ -4521,7 +4552,7 @@
       <c r="D55" s="39"/>
       <c r="E55" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F55" s="31"/>
       <c r="G55" s="2"/>
@@ -4532,7 +4563,7 @@
       <c r="D56" s="39"/>
       <c r="E56" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F56" s="31"/>
       <c r="G56" s="2"/>
@@ -4543,7 +4574,7 @@
       <c r="D57" s="39"/>
       <c r="E57" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F57" s="31"/>
       <c r="G57" s="2"/>
@@ -4554,7 +4585,7 @@
       <c r="D58" s="39"/>
       <c r="E58" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F58" s="31"/>
       <c r="G58" s="2"/>
@@ -4565,7 +4596,7 @@
       <c r="D59" s="39"/>
       <c r="E59" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F59" s="31"/>
       <c r="G59" s="2"/>
@@ -4576,7 +4607,7 @@
       <c r="D60" s="39"/>
       <c r="E60" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F60" s="31"/>
       <c r="G60" s="2"/>
@@ -4587,7 +4618,7 @@
       <c r="D61" s="39"/>
       <c r="E61" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F61" s="31"/>
       <c r="G61" s="2"/>
@@ -4598,7 +4629,7 @@
       <c r="D62" s="39"/>
       <c r="E62" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F62" s="31"/>
       <c r="G62" s="2"/>
@@ -4609,7 +4640,7 @@
       <c r="D63" s="39"/>
       <c r="E63" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F63" s="31"/>
       <c r="G63" s="2"/>
@@ -4620,7 +4651,7 @@
       <c r="D64" s="39"/>
       <c r="E64" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F64" s="31"/>
       <c r="G64" s="2"/>
@@ -4631,7 +4662,7 @@
       <c r="D65" s="39"/>
       <c r="E65" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F65" s="31"/>
       <c r="G65" s="2"/>
@@ -4642,7 +4673,7 @@
       <c r="D66" s="39"/>
       <c r="E66" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F66" s="31"/>
       <c r="G66" s="2"/>
@@ -4653,7 +4684,7 @@
       <c r="D67" s="39"/>
       <c r="E67" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F67" s="31"/>
       <c r="G67" s="2"/>
@@ -4664,7 +4695,7 @@
       <c r="D68" s="39"/>
       <c r="E68" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F68" s="31"/>
       <c r="G68" s="2"/>
@@ -4675,7 +4706,7 @@
       <c r="D69" s="39"/>
       <c r="E69" s="41">
         <f t="shared" si="1"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F69" s="31"/>
       <c r="G69" s="2"/>
@@ -4686,7 +4717,7 @@
       <c r="D70" s="39"/>
       <c r="E70" s="41">
         <f t="shared" ref="E70:E82" si="2">E69+C70-D70</f>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F70" s="31"/>
       <c r="G70" s="2"/>
@@ -4697,7 +4728,7 @@
       <c r="D71" s="39"/>
       <c r="E71" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F71" s="31"/>
       <c r="G71" s="2"/>
@@ -4708,7 +4739,7 @@
       <c r="D72" s="39"/>
       <c r="E72" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F72" s="31"/>
       <c r="G72" s="2"/>
@@ -4719,7 +4750,7 @@
       <c r="D73" s="39"/>
       <c r="E73" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F73" s="31"/>
       <c r="G73" s="2"/>
@@ -4730,7 +4761,7 @@
       <c r="D74" s="39"/>
       <c r="E74" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F74" s="31"/>
       <c r="G74" s="2"/>
@@ -4741,7 +4772,7 @@
       <c r="D75" s="39"/>
       <c r="E75" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F75" s="33"/>
       <c r="G75" s="2"/>
@@ -4752,7 +4783,7 @@
       <c r="D76" s="39"/>
       <c r="E76" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F76" s="31"/>
       <c r="G76" s="2"/>
@@ -4763,7 +4794,7 @@
       <c r="D77" s="39"/>
       <c r="E77" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F77" s="31"/>
       <c r="G77" s="2"/>
@@ -4774,7 +4805,7 @@
       <c r="D78" s="39"/>
       <c r="E78" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F78" s="31"/>
       <c r="G78" s="2"/>
@@ -4785,7 +4816,7 @@
       <c r="D79" s="39"/>
       <c r="E79" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F79" s="31"/>
       <c r="G79" s="2"/>
@@ -4796,7 +4827,7 @@
       <c r="D80" s="39"/>
       <c r="E80" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F80" s="31"/>
       <c r="G80" s="2"/>
@@ -4807,7 +4838,7 @@
       <c r="D81" s="39"/>
       <c r="E81" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F81" s="31"/>
       <c r="G81" s="2"/>
@@ -4818,7 +4849,7 @@
       <c r="D82" s="39"/>
       <c r="E82" s="41">
         <f t="shared" si="2"/>
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F82" s="31"/>
       <c r="G82" s="2"/>
@@ -4827,15 +4858,15 @@
       <c r="B83" s="45"/>
       <c r="C83" s="41">
         <f>SUM(C5:C72)</f>
-        <v>11476844</v>
+        <v>11976844</v>
       </c>
       <c r="D83" s="41">
         <f>SUM(D5:D77)</f>
-        <v>9500000</v>
+        <v>9900000</v>
       </c>
       <c r="E83" s="66">
         <f>E71+C83-D83</f>
-        <v>3953688</v>
+        <v>4153688</v>
       </c>
       <c r="F83" s="32"/>
       <c r="G83" s="2"/>
@@ -4863,8 +4894,8 @@
   </sheetPr>
   <dimension ref="A1:AC222"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4968,7 +4999,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="72">
-        <v>2049618.9539999999</v>
+        <v>2535365.8759999997</v>
       </c>
       <c r="F4" s="63"/>
       <c r="G4" s="55"/>
@@ -5000,14 +5031,14 @@
         <v>6</v>
       </c>
       <c r="B5" s="71">
-        <v>215323.01</v>
+        <v>230732.55000000005</v>
       </c>
       <c r="C5" s="71"/>
       <c r="D5" s="68" t="s">
         <v>23</v>
       </c>
       <c r="E5" s="72">
-        <v>1976844</v>
+        <v>2076844</v>
       </c>
       <c r="F5" s="5"/>
       <c r="G5" s="55"/>
@@ -5040,14 +5071,14 @@
       </c>
       <c r="B6" s="71">
         <f>B4+B5</f>
-        <v>8716064.0099999998</v>
+        <v>8731473.5500000007</v>
       </c>
       <c r="C6" s="68"/>
       <c r="D6" s="68" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="289">
-        <v>503220</v>
+        <v>670417</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="55"/>
@@ -5084,7 +5115,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="73">
-        <v>2443876</v>
+        <v>2423126</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="55"/>
@@ -5116,7 +5147,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="71">
-        <v>33511</v>
+        <v>36379</v>
       </c>
       <c r="C8" s="70"/>
       <c r="D8" s="68" t="s">
@@ -5195,14 +5226,14 @@
       </c>
       <c r="B10" s="75">
         <f>B5-B8-B9</f>
-        <v>181812.01</v>
+        <v>194353.55000000005</v>
       </c>
       <c r="C10" s="70"/>
       <c r="D10" s="68" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="73">
-        <v>1563945.0559999999</v>
+        <v>844292.67400000058</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="50"/>
@@ -5309,7 +5340,7 @@
       </c>
       <c r="B13" s="74">
         <f>B6-B8-B11+B12-B9</f>
-        <v>8632553.0099999998</v>
+        <v>8645094.5500000007</v>
       </c>
       <c r="C13" s="70"/>
       <c r="D13" s="70" t="s">
@@ -5317,7 +5348,7 @@
       </c>
       <c r="E13" s="73">
         <f>E4+E5+E6+E7+E8+E9+E10</f>
-        <v>8632553.0099999998</v>
+        <v>8645094.5500000007</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="290">
@@ -5606,7 +5637,7 @@
     </row>
     <row r="21" spans="1:29" ht="20.25">
       <c r="A21" s="59" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B21" s="53">
         <v>48895</v>
@@ -5647,7 +5678,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="53">
-        <v>412890</v>
+        <v>390890</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="19" t="s">
@@ -5685,7 +5716,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="92">
-        <v>287296</v>
+        <v>267296</v>
       </c>
       <c r="C23" s="93"/>
       <c r="D23" s="94" t="s">
@@ -10575,7 +10606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BI246"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A101" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
@@ -11770,7 +11801,7 @@
     </row>
     <row r="17" spans="1:61" ht="12.6" customHeight="1">
       <c r="A17" s="114" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B17" s="115">
         <v>807380</v>
@@ -11846,7 +11877,7 @@
     </row>
     <row r="18" spans="1:61" ht="12.6" customHeight="1">
       <c r="A18" s="114" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B18" s="115">
         <v>791090</v>
@@ -11922,7 +11953,7 @@
     </row>
     <row r="19" spans="1:61" ht="12.6" customHeight="1">
       <c r="A19" s="114" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B19" s="115">
         <v>515085</v>
@@ -11997,13 +12028,21 @@
       <c r="BI19" s="105"/>
     </row>
     <row r="20" spans="1:61" ht="12.6" customHeight="1">
-      <c r="A20" s="114"/>
-      <c r="B20" s="115"/>
-      <c r="C20" s="115"/>
-      <c r="D20" s="115"/>
+      <c r="A20" s="114" t="s">
+        <v>220</v>
+      </c>
+      <c r="B20" s="115">
+        <v>651405</v>
+      </c>
+      <c r="C20" s="115">
+        <v>669387</v>
+      </c>
+      <c r="D20" s="115">
+        <v>2768</v>
+      </c>
       <c r="E20" s="115">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>672155</v>
       </c>
       <c r="F20" s="116"/>
       <c r="G20" s="104"/>
@@ -12884,23 +12923,23 @@
       </c>
       <c r="B33" s="115">
         <f>SUM(B5:B32)</f>
-        <v>9081470</v>
+        <v>9732875</v>
       </c>
       <c r="C33" s="115">
         <f>SUM(C5:C32)</f>
-        <v>8911910</v>
+        <v>9581297</v>
       </c>
       <c r="D33" s="115">
         <f>SUM(D5:D32)</f>
-        <v>32531</v>
+        <v>35299</v>
       </c>
       <c r="E33" s="115">
         <f>SUM(E5:E32)</f>
-        <v>8944441</v>
+        <v>9616596</v>
       </c>
       <c r="F33" s="123">
         <f>B33-E33</f>
-        <v>137029</v>
+        <v>116279</v>
       </c>
       <c r="G33" s="137"/>
       <c r="H33" s="145"/>
@@ -13316,7 +13355,7 @@
         <v>4000</v>
       </c>
       <c r="D39" s="155" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E39" s="120"/>
       <c r="F39" s="116"/>
@@ -13455,10 +13494,10 @@
         <v>60</v>
       </c>
       <c r="C41" s="115">
-        <v>24750</v>
+        <v>26750</v>
       </c>
       <c r="D41" s="108" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E41" s="159"/>
       <c r="F41" s="116"/>
@@ -13529,7 +13568,7 @@
         <v>1580</v>
       </c>
       <c r="D42" s="108" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F42" s="162"/>
       <c r="G42" s="163"/>
@@ -13596,10 +13635,10 @@
         <v>206</v>
       </c>
       <c r="C43" s="115">
-        <v>23500</v>
+        <v>24500</v>
       </c>
       <c r="D43" s="108" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E43" s="121"/>
       <c r="F43" s="324" t="s">
@@ -13995,7 +14034,7 @@
       </c>
       <c r="B49" s="185"/>
       <c r="C49" s="184">
-        <v>287297</v>
+        <v>267297</v>
       </c>
       <c r="D49" s="185" t="s">
         <v>220</v>
@@ -14131,7 +14170,7 @@
       </c>
       <c r="B51" s="112"/>
       <c r="C51" s="184">
-        <v>85380</v>
+        <v>85250</v>
       </c>
       <c r="D51" s="188" t="s">
         <v>220</v>
@@ -14272,7 +14311,7 @@
         <v>414940</v>
       </c>
       <c r="D53" s="191" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E53" s="120"/>
       <c r="F53" s="113"/>
@@ -14338,10 +14377,10 @@
       </c>
       <c r="B54" s="112"/>
       <c r="C54" s="184">
-        <v>189605</v>
+        <v>190455</v>
       </c>
       <c r="D54" s="180" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E54" s="120"/>
       <c r="F54" s="144"/>
@@ -14410,7 +14449,7 @@
         <v>9000</v>
       </c>
       <c r="D55" s="191" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E55" s="120"/>
       <c r="F55" s="112"/>
@@ -14476,10 +14515,10 @@
       </c>
       <c r="B56" s="112"/>
       <c r="C56" s="184">
-        <v>10000</v>
+        <v>21000</v>
       </c>
       <c r="D56" s="188" t="s">
-        <v>207</v>
+        <v>220</v>
       </c>
       <c r="E56" s="120"/>
       <c r="F56" s="112"/>
@@ -15360,7 +15399,7 @@
         <v>23800</v>
       </c>
       <c r="D68" s="191" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E68" s="120"/>
       <c r="F68" s="196"/>
@@ -16786,16 +16825,10 @@
       <c r="BI85" s="105"/>
     </row>
     <row r="86" spans="1:61" ht="12.75" customHeight="1">
-      <c r="A86" s="187" t="s">
-        <v>214</v>
-      </c>
+      <c r="A86" s="187"/>
       <c r="B86" s="112"/>
-      <c r="C86" s="184">
-        <v>2000</v>
-      </c>
-      <c r="D86" s="188" t="s">
-        <v>213</v>
-      </c>
+      <c r="C86" s="184"/>
+      <c r="D86" s="188"/>
       <c r="E86" s="121"/>
       <c r="F86" s="203"/>
       <c r="G86" s="197" t="s">
@@ -16867,14 +16900,14 @@
     </row>
     <row r="87" spans="1:61" ht="12.75" customHeight="1">
       <c r="A87" s="187" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B87" s="112"/>
       <c r="C87" s="287">
         <v>9000</v>
       </c>
       <c r="D87" s="188" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E87" s="120"/>
       <c r="F87" s="203"/>
@@ -17021,14 +17054,14 @@
     </row>
     <row r="89" spans="1:61" ht="12.75" customHeight="1">
       <c r="A89" s="187" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B89" s="185"/>
       <c r="C89" s="184">
         <v>2160</v>
       </c>
       <c r="D89" s="191" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E89" s="120"/>
       <c r="F89" s="203"/>
@@ -17100,16 +17133,10 @@
       <c r="BI89" s="105"/>
     </row>
     <row r="90" spans="1:61" ht="12.6" customHeight="1">
-      <c r="A90" s="187" t="s">
-        <v>215</v>
-      </c>
+      <c r="A90" s="187"/>
       <c r="B90" s="185"/>
-      <c r="C90" s="184">
-        <v>13470</v>
-      </c>
-      <c r="D90" s="185" t="s">
-        <v>213</v>
-      </c>
+      <c r="C90" s="184"/>
+      <c r="D90" s="185"/>
       <c r="E90" s="120"/>
       <c r="F90" s="203"/>
       <c r="G90" s="197" t="s">
@@ -17948,7 +17975,7 @@
         <v>204</v>
       </c>
       <c r="B101" s="294" t="s">
-        <v>127</v>
+        <v>222</v>
       </c>
       <c r="C101" s="295">
         <v>570</v>
@@ -18172,7 +18199,7 @@
         <v>2340</v>
       </c>
       <c r="D104" s="185" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F104" s="207"/>
       <c r="G104" s="201"/>
@@ -18316,7 +18343,7 @@
         <v>17500</v>
       </c>
       <c r="D106" s="188" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F106" s="207"/>
       <c r="G106" s="201"/>
@@ -18824,7 +18851,7 @@
       <c r="B113" s="314"/>
       <c r="C113" s="210">
         <f>SUM(C37:C112)</f>
-        <v>2443876</v>
+        <v>2423126</v>
       </c>
       <c r="D113" s="211"/>
       <c r="F113" s="203"/>
@@ -18969,7 +18996,7 @@
       <c r="B115" s="316"/>
       <c r="C115" s="215">
         <f>C113+L136</f>
-        <v>2443876</v>
+        <v>2423126</v>
       </c>
       <c r="D115" s="216"/>
       <c r="F115" s="196"/>
@@ -21696,11 +21723,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Z321"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10" ySplit="14" topLeftCell="K15" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="10" ySplit="14" topLeftCell="K35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="N23" sqref="N23"/>
+      <selection pane="bottomRight" activeCell="S38" sqref="S38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -22429,7 +22456,7 @@
     </row>
     <row r="19" spans="1:25" s="22" customFormat="1">
       <c r="A19" s="248" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B19" s="256"/>
       <c r="C19" s="249">
@@ -22471,7 +22498,7 @@
     </row>
     <row r="20" spans="1:25" s="22" customFormat="1">
       <c r="A20" s="248" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B20" s="256">
         <v>800</v>
@@ -22513,7 +22540,7 @@
     </row>
     <row r="21" spans="1:25" s="22" customFormat="1">
       <c r="A21" s="248" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B21" s="256">
         <v>1600</v>
@@ -22523,7 +22550,7 @@
         <v>155</v>
       </c>
       <c r="E21" s="257"/>
-      <c r="F21" s="257"/>
+      <c r="F21" s="297"/>
       <c r="G21" s="257">
         <v>360</v>
       </c>
@@ -22554,27 +22581,41 @@
       <c r="Y21" s="5"/>
     </row>
     <row r="22" spans="1:25" s="22" customFormat="1">
-      <c r="A22" s="248"/>
-      <c r="B22" s="256"/>
+      <c r="A22" s="248" t="s">
+        <v>220</v>
+      </c>
+      <c r="B22" s="256">
+        <v>1000</v>
+      </c>
       <c r="C22" s="249"/>
       <c r="D22" s="257"/>
       <c r="E22" s="257"/>
-      <c r="F22" s="257"/>
-      <c r="G22" s="257"/>
+      <c r="F22" s="257">
+        <v>1138</v>
+      </c>
+      <c r="G22" s="257">
+        <v>110</v>
+      </c>
       <c r="H22" s="257"/>
       <c r="I22" s="257"/>
-      <c r="J22" s="257"/>
-      <c r="K22" s="257"/>
+      <c r="J22" s="257">
+        <v>20</v>
+      </c>
+      <c r="K22" s="257">
+        <v>480</v>
+      </c>
       <c r="L22" s="257"/>
       <c r="M22" s="257"/>
-      <c r="N22" s="297"/>
+      <c r="N22" s="297">
+        <v>20</v>
+      </c>
       <c r="O22" s="257"/>
       <c r="P22" s="257"/>
       <c r="Q22" s="257"/>
       <c r="R22" s="259"/>
       <c r="S22" s="253">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2768</v>
       </c>
       <c r="T22" s="254"/>
       <c r="U22" s="7"/>
@@ -22980,7 +23021,7 @@
       </c>
       <c r="B38" s="274">
         <f>SUM(B7:B37)</f>
-        <v>13400</v>
+        <v>14400</v>
       </c>
       <c r="C38" s="275">
         <f t="shared" ref="C38:R38" si="1">SUM(C7:C37)</f>
@@ -22996,11 +23037,11 @@
       </c>
       <c r="F38" s="275">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1138</v>
       </c>
       <c r="G38" s="275">
         <f>SUM(G7:G37)</f>
-        <v>4340</v>
+        <v>4450</v>
       </c>
       <c r="H38" s="275">
         <f t="shared" si="1"/>
@@ -23012,11 +23053,11 @@
       </c>
       <c r="J38" s="275">
         <f t="shared" si="1"/>
-        <v>390</v>
+        <v>410</v>
       </c>
       <c r="K38" s="275">
         <f t="shared" si="1"/>
-        <v>7100</v>
+        <v>7580</v>
       </c>
       <c r="L38" s="275">
         <f t="shared" si="1"/>
@@ -23028,7 +23069,7 @@
       </c>
       <c r="N38" s="300">
         <f t="shared" si="1"/>
-        <v>460</v>
+        <v>480</v>
       </c>
       <c r="O38" s="275">
         <f t="shared" si="1"/>
@@ -23048,7 +23089,7 @@
       </c>
       <c r="S38" s="277">
         <f>SUM(S7:S37)</f>
-        <v>33611</v>
+        <v>36379</v>
       </c>
     </row>
     <row r="39" spans="1:20">

</xml_diff>